<commit_message>
tahara naksha complete of ram bahadur karki and expense updated
</commit_message>
<xml_diff>
--- a/ofc/expense.xlsx
+++ b/ofc/expense.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -43,10 +43,13 @@
     <t>Thyroid test</t>
   </si>
   <si>
-    <t>chiya samosa</t>
-  </si>
-  <si>
     <t>tire haawa haleko, Roforty-F medicine for helping get pregnant, daxhina to aacha baju</t>
+  </si>
+  <si>
+    <t>dinesh vinaju &amp; prabin chiya, irika bus fare, Photocopy, apple, chocolate</t>
+  </si>
+  <si>
+    <t>Petrol, chiya samosa</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,7 +520,7 @@
         <v>66429</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
         <f>10+1620+5+10</f>
@@ -541,24 +544,34 @@
       <c r="A5" s="4">
         <v>66431</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5">
-        <v>100</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="4">
+        <v>66432</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
+        <f>150+100</f>
+        <v>250</v>
+      </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>66433</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5">
+        <f>65+100+50+325+50</f>
+        <v>590</v>
+      </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
expense update upto 2025/03/04
</commit_message>
<xml_diff>
--- a/ofc/expense.xlsx
+++ b/ofc/expense.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Petrol, chiya samosa</t>
+  </si>
+  <si>
+    <t>chiya patti 1pau, biscuit 1 packet, advance for asset ring</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,9 +578,16 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="4">
+        <v>66434</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5">
+        <f>110+80+10000</f>
+        <v>10190</v>
+      </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
expense and sh include
</commit_message>
<xml_diff>
--- a/ofc/expense.xlsx
+++ b/ofc/expense.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -46,13 +46,16 @@
     <t>tire haawa haleko, Roforty-F medicine for helping get pregnant, daxhina to aacha baju</t>
   </si>
   <si>
-    <t>dinesh vinaju &amp; prabin chiya, irika bus fare, Photocopy, apple, chocolate</t>
-  </si>
-  <si>
     <t>Petrol, chiya samosa</t>
   </si>
   <si>
     <t>chiya patti 1pau, biscuit 1 packet, advance for asset ring</t>
+  </si>
+  <si>
+    <t>folic acid, bal krishna sir</t>
+  </si>
+  <si>
+    <t>dinesh vinaju &amp; prabin chiya, irika bus fare, Photocopy, apple, chocolate, bal krishna sir</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +559,7 @@
         <v>66432</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5">
         <f>150+100</f>
@@ -569,11 +572,11 @@
         <v>66433</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5">
-        <f>65+100+50+325+50</f>
-        <v>590</v>
+        <f>65+100+50+325+50+1000</f>
+        <v>1590</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -582,7 +585,7 @@
         <v>66434</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5">
         <f>110+80+10000</f>
@@ -591,19 +594,30 @@
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="4">
+        <v>66435</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5">
+        <f>30+1000</f>
+        <v>1030</v>
+      </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="4">
+        <v>66436</v>
+      </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="4">
+        <v>66437</v>
+      </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>

</xml_diff>